<commit_message>
amazon - test cases
</commit_message>
<xml_diff>
--- a/Amazon - Test Cases for To Add an Address and Buy A Product.xlsx
+++ b/Amazon - Test Cases for To Add an Address and Buy A Product.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Buy a product - test case" sheetId="1" r:id="rId1"/>
     <sheet name="Add an address-test case" sheetId="4" r:id="rId2"/>
+    <sheet name="Order Tracking" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>Scenario No</t>
   </si>
@@ -197,6 +198,54 @@
   <si>
     <t>Validate the 'add an address' 
 option to update new address</t>
+  </si>
+  <si>
+    <t>Validate the 'Buy A Product'
+ through 'UPI'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test description
+validate if the product is successfully place to order through UPI option
+precondition:
+user has access to the URL
+</t>
+  </si>
+  <si>
+    <t>click on 'UPI' radiobutton in payment section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seelct the UPI apps in drop down option and enter UPI id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the blue color highlighted 
+in the text box and displays the UPI id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">click 'pay seurely' option </t>
+  </si>
+  <si>
+    <t>click on 'Cash On Delivery' radiobutton in payment section</t>
+  </si>
+  <si>
+    <t>Validate the 'Buy A Product'
+ through 'Cash On Delivery'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test description
+validate if the product is successfully place to order through Cash on Delivery option
+precondition:
+user has access to the URL
+</t>
+  </si>
+  <si>
+    <t>the UPI app is displayed to pay.the message is diplayed 'your order is sucesssfully placed'</t>
+  </si>
+  <si>
+    <t>click on 'Place Your Order' option</t>
+  </si>
+  <si>
+    <t>the message is dislayed 'your
+ order is successfully placed.</t>
   </si>
 </sst>
 </file>
@@ -310,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -352,6 +401,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -666,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -729,10 +789,10 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="43.2">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="3">
         <v>2</v>
       </c>
@@ -744,10 +804,10 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="28.8">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="13"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="3">
         <v>3</v>
       </c>
@@ -759,10 +819,10 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="28.8">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="13"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="3">
         <v>4</v>
       </c>
@@ -774,10 +834,10 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="43.2">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="13"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="3">
         <v>5</v>
       </c>
@@ -789,10 +849,10 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="28.8">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="13"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="3">
         <v>6</v>
       </c>
@@ -804,10 +864,10 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="28.8">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="3">
         <v>7</v>
       </c>
@@ -819,10 +879,10 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="28.8">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="3">
         <v>8</v>
       </c>
@@ -834,10 +894,10 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="43.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="3">
         <v>9</v>
       </c>
@@ -849,10 +909,10 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.8">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="3">
         <v>10</v>
       </c>
@@ -864,10 +924,10 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="28.8">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="3">
         <v>11</v>
       </c>
@@ -879,16 +939,337 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="14"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="3"/>
     </row>
+    <row r="14" spans="2:8" ht="28.8" customHeight="1">
+      <c r="B14" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="43.2">
+      <c r="B15" s="10"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="28.8">
+      <c r="B16" s="10"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="28.8">
+      <c r="B17" s="10"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="3">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="43.2">
+      <c r="B18" s="10"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="3">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="28.8">
+      <c r="B19" s="10"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="3">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="28.8">
+      <c r="B20" s="10"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="3">
+        <v>7</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="28.8">
+      <c r="B21" s="10"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="3">
+        <v>8</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="28.8">
+      <c r="B22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="3">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="43.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="3">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="28.8" customHeight="1">
+      <c r="B24" s="9">
+        <v>1.3</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="28.8" customHeight="1">
+      <c r="B25" s="10"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="28.8">
+      <c r="B26" s="10"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="3">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="28.8">
+      <c r="B27" s="10"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="43.2">
+      <c r="B28" s="10"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="3">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="28.8">
+      <c r="B29" s="10"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="3">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="28.8">
+      <c r="B30" s="10"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="3">
+        <v>7</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="28.8">
+      <c r="B31" s="10"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="3">
+        <v>8</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="28.8">
+      <c r="B32" s="11"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="3">
+        <v>9</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="17"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
+    <mergeCell ref="E14:E23"/>
+    <mergeCell ref="D14:D23"/>
+    <mergeCell ref="C14:C23"/>
+    <mergeCell ref="B14:B23"/>
+    <mergeCell ref="C24:C32"/>
+    <mergeCell ref="D24:D32"/>
+    <mergeCell ref="E24:E32"/>
+    <mergeCell ref="B24:B32"/>
     <mergeCell ref="D2:D13"/>
     <mergeCell ref="E2:E13"/>
     <mergeCell ref="C2:C13"/>
@@ -902,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -1152,4 +1533,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>